<commit_message>
Almost finished with project writeup
</commit_message>
<xml_diff>
--- a/Data/Records/blob statistics.xlsx
+++ b/Data/Records/blob statistics.xlsx
@@ -4,10 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24526"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-23020" yWindow="2280" windowWidth="19240" windowHeight="13520" tabRatio="500"/>
+    <workbookView xWindow="6120" yWindow="140" windowWidth="20480" windowHeight="16760" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Statistics" sheetId="2" r:id="rId1"/>
+    <sheet name="Confusion" sheetId="3" r:id="rId2"/>
+    <sheet name="Different Lighting" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="Hu_Descriptor_Comparison" localSheetId="0">Statistics!$C$5:$L$59</definedName>
@@ -24,7 +26,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <connection id="1" name="Hu Descriptor Comparison.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:donj:workspace:Morphology:Data:Records:Hu Descriptor Comparison.txt" tab="0" space="1" consecutive="1">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:donj:workspace:Morphology:Data:Records:Hu Descriptor Comparison.txt" tab="0" space="1" consecutive="1">
       <textFields count="7">
         <textField/>
         <textField/>
@@ -37,14 +39,14 @@
     </textPr>
   </connection>
   <connection id="2" name="log.txt" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:donj:workspace:Morphology:Data:Output:log.txt">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:donj:workspace:Morphology:Data:Output:log.txt">
       <textFields>
         <textField/>
       </textFields>
     </textPr>
   </connection>
   <connection id="3" name="log.txt1" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:donj:workspace:Morphology:Data:Output:log.txt" delimited="0">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:donj:workspace:Morphology:Data:Output:log.txt" delimited="0">
       <textFields count="14">
         <textField/>
         <textField position="2"/>
@@ -64,7 +66,7 @@
     </textPr>
   </connection>
   <connection id="4" name="log.txt2" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:donj:workspace:Morphology:Data:Output:log.txt">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:donj:workspace:Morphology:Data:Output:log.txt">
       <textFields count="11">
         <textField/>
         <textField/>
@@ -81,7 +83,7 @@
     </textPr>
   </connection>
   <connection id="5" name="log.txt3" type="6" refreshedVersion="0" background="1" saveData="1">
-    <textPr fileType="mac" codePage="10000" sourceFile="Macintosh HD:Users:donj:workspace:Morphology:Data:Output:log.txt">
+    <textPr fileType="mac" sourceFile="Macintosh HD:Users:donj:workspace:Morphology:Data:Output:log.txt">
       <textFields count="11">
         <textField/>
         <textField/>
@@ -101,7 +103,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="63">
   <si>
     <t>Forks</t>
   </si>
@@ -167,13 +169,136 @@
   </si>
   <si>
     <t>(Knife+Fork Compactness)/2</t>
+  </si>
+  <si>
+    <t>Unknowns</t>
+  </si>
+  <si>
+    <t>Run</t>
+  </si>
+  <si>
+    <t>Application Classified</t>
+  </si>
+  <si>
+    <t>Ground Truth</t>
+  </si>
+  <si>
+    <t>DSC02141</t>
+  </si>
+  <si>
+    <t>DSC02142</t>
+  </si>
+  <si>
+    <t>DSC02143</t>
+  </si>
+  <si>
+    <t>DSC02144</t>
+  </si>
+  <si>
+    <t>DSC02145</t>
+  </si>
+  <si>
+    <t>DSC02146</t>
+  </si>
+  <si>
+    <t>DSC02147</t>
+  </si>
+  <si>
+    <t>DSC02148</t>
+  </si>
+  <si>
+    <t>DSC02158</t>
+  </si>
+  <si>
+    <t>DSC02138</t>
+  </si>
+  <si>
+    <t>DSC02149</t>
+  </si>
+  <si>
+    <t>DSC02157</t>
+  </si>
+  <si>
+    <t>DSC02159</t>
+  </si>
+  <si>
+    <t>DSC02160</t>
+  </si>
+  <si>
+    <t>DSC02161</t>
+  </si>
+  <si>
+    <t>DSC02162</t>
+  </si>
+  <si>
+    <t>DSC02166</t>
+  </si>
+  <si>
+    <t>DSC02167</t>
+  </si>
+  <si>
+    <t>DSC02168</t>
+  </si>
+  <si>
+    <t>DSC02169</t>
+  </si>
+  <si>
+    <t>DSC02170</t>
+  </si>
+  <si>
+    <t>DSC02173</t>
+  </si>
+  <si>
+    <t>DSC02171</t>
+  </si>
+  <si>
+    <t>DSC02175</t>
+  </si>
+  <si>
+    <t>DSC02174</t>
+  </si>
+  <si>
+    <t>DSC02176</t>
+  </si>
+  <si>
+    <t>DSC02177</t>
+  </si>
+  <si>
+    <t>DSC02178</t>
+  </si>
+  <si>
+    <t>DSC02179</t>
+  </si>
+  <si>
+    <t>Summary</t>
+  </si>
+  <si>
+    <t>Confusion Matrix for Full Automated Operation of Count Objects Application</t>
+  </si>
+  <si>
+    <t>DSC02172</t>
+  </si>
+  <si>
+    <t>Acurracy</t>
+  </si>
+  <si>
+    <t>Incorrect</t>
+  </si>
+  <si>
+    <t>Correct</t>
+  </si>
+  <si>
+    <t>&lt;---- Reference image for selecting background classes</t>
+  </si>
+  <si>
+    <t>Application Classifications</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -238,16 +363,42 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF8DB4E2"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -255,8 +406,121 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="155">
+  <cellStyleXfs count="249">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -412,8 +676,102 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
@@ -446,8 +804,46 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="155">
+  <cellStyles count="249">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -525,6 +921,53 @@
     <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="244" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="246" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="248" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -602,6 +1045,53 @@
     <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="243" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="245" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="247" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -937,7 +1427,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
@@ -1795,35 +2285,35 @@
     <row r="28" spans="1:15">
       <c r="C28" s="3"/>
       <c r="D28" s="8">
-        <f>AVERAGE(D21:D27)</f>
+        <f t="shared" ref="D28:K28" si="3">AVERAGE(D21:D27)</f>
         <v>1.0610109999999999</v>
       </c>
       <c r="E28" s="8">
-        <f>AVERAGE(E21:E27)</f>
+        <f t="shared" si="3"/>
         <v>1.0391598333333334</v>
       </c>
       <c r="F28" s="8">
-        <f>AVERAGE(F21:F27)</f>
+        <f t="shared" si="3"/>
         <v>0.47705850000000005</v>
       </c>
       <c r="G28" s="8">
-        <f>AVERAGE(G21:G27)</f>
+        <f t="shared" si="3"/>
         <v>0.41364816666666665</v>
       </c>
       <c r="H28" s="8">
-        <f>AVERAGE(H21:H27)</f>
+        <f t="shared" si="3"/>
         <v>0.18726083333333332</v>
       </c>
       <c r="I28" s="8">
-        <f>AVERAGE(I21:I27)</f>
+        <f t="shared" si="3"/>
         <v>0.42340116666666666</v>
       </c>
       <c r="J28" s="8">
-        <f>AVERAGE(J21:J27)</f>
+        <f t="shared" si="3"/>
         <v>4.8000000000000001E-5</v>
       </c>
       <c r="K28" s="8">
-        <f>AVERAGE(K21:K27)</f>
+        <f t="shared" si="3"/>
         <v>-4.1592499999999998E-3</v>
       </c>
       <c r="L28" s="8">
@@ -2207,23 +2697,23 @@
         <v>1.2943105714285714</v>
       </c>
       <c r="E43" s="8">
-        <f t="shared" ref="E43:I43" si="3">AVERAGE(E35:E42)</f>
+        <f t="shared" ref="E43:I43" si="4">AVERAGE(E35:E42)</f>
         <v>1.6478764285714285</v>
       </c>
       <c r="F43" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.913642857142857E-2</v>
       </c>
       <c r="G43" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>9.2800571428571427E-2</v>
       </c>
       <c r="H43" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1.3330571428571428E-2</v>
       </c>
       <c r="I43" s="8">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>0.12494414285714285</v>
       </c>
       <c r="J43" s="8"/>
@@ -2718,4 +3208,1574 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K142"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="9.1640625" customWidth="1"/>
+    <col min="2" max="2" width="11" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" customWidth="1"/>
+    <col min="10" max="11" width="22.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:11">
+      <c r="A1" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="4" spans="1:11">
+      <c r="A4" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="C4" s="27"/>
+      <c r="D4" s="28"/>
+      <c r="E4" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="30"/>
+    </row>
+    <row r="5" spans="1:11">
+      <c r="C5" s="31"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="F5" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G5" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="H5" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
+      <c r="C6" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E6" s="32">
+        <f>SUM(E15+E22+E29+E36+E43+E50+E57+E64+E71)</f>
+        <v>13</v>
+      </c>
+      <c r="F6" s="32">
+        <f t="shared" ref="F6:H6" si="0">SUM(F15+F22+F29+F36+F43+F50+F57+F64+F71)</f>
+        <v>0</v>
+      </c>
+      <c r="G6" s="32">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H6" s="32">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="J6" t="s">
+        <v>59</v>
+      </c>
+      <c r="K6">
+        <f>SUM(E7+E8+E9+F6+F8+F9+G6+G7+G9+H6+H7+H8)</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
+      <c r="C7" s="34"/>
+      <c r="D7" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E7" s="32">
+        <f>SUM(E16+E23+E30+E37+E44+E51+E58+E65+E72)</f>
+        <v>0</v>
+      </c>
+      <c r="F7" s="32">
+        <f t="shared" ref="F7:H7" si="1">SUM(F16+F23+F30+F37+F44+F51+F58+F65+F72)</f>
+        <v>12</v>
+      </c>
+      <c r="G7" s="32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H7" s="32">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K7">
+        <f>SUM(E6+F7+G8+H9)</f>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
+      <c r="C8" s="34"/>
+      <c r="D8" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="32">
+        <f t="shared" ref="E8:H9" si="2">SUM(E17+E24+E31+E38+E45+E52+E59+E66+E73)</f>
+        <v>0</v>
+      </c>
+      <c r="F8" s="32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G8" s="32">
+        <f t="shared" si="2"/>
+        <v>14</v>
+      </c>
+      <c r="H8" s="32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="J8" s="39" t="s">
+        <v>58</v>
+      </c>
+      <c r="K8" s="40">
+        <f>(K7-K6)/K7</f>
+        <v>0.96969696969696972</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
+      <c r="C9" s="38"/>
+      <c r="D9" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E9" s="32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F9" s="32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="32">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="32">
+        <f t="shared" si="2"/>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
+      <c r="A11" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B11" s="4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
+      <c r="A13" s="18">
+        <v>1</v>
+      </c>
+      <c r="B13" t="s">
+        <v>48</v>
+      </c>
+      <c r="C13" s="27"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F13" s="29"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="30"/>
+      <c r="J13" s="41" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="C14" s="31"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="F14" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G14" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
+      <c r="C15" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D15" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E15" s="32">
+        <v>2</v>
+      </c>
+      <c r="F15" s="32">
+        <v>0</v>
+      </c>
+      <c r="G15" s="32">
+        <v>0</v>
+      </c>
+      <c r="H15" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
+      <c r="C16" s="34"/>
+      <c r="D16" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E16" s="32">
+        <v>0</v>
+      </c>
+      <c r="F16" s="32">
+        <v>1</v>
+      </c>
+      <c r="G16" s="32">
+        <v>0</v>
+      </c>
+      <c r="H16" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="C17" s="34"/>
+      <c r="D17" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E17" s="32">
+        <v>0</v>
+      </c>
+      <c r="F17" s="32">
+        <v>0</v>
+      </c>
+      <c r="G17" s="32">
+        <v>2</v>
+      </c>
+      <c r="H17" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="C18" s="38"/>
+      <c r="D18" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18" s="32">
+        <v>0</v>
+      </c>
+      <c r="F18" s="32">
+        <v>0</v>
+      </c>
+      <c r="G18" s="32">
+        <v>0</v>
+      </c>
+      <c r="H18" s="32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="18">
+        <v>2</v>
+      </c>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" s="27"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F20" s="29"/>
+      <c r="G20" s="29"/>
+      <c r="H20" s="30"/>
+    </row>
+    <row r="21" spans="1:8">
+      <c r="C21" s="31"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="F21" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="H21" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8">
+      <c r="C22" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D22" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E22" s="32">
+        <v>1</v>
+      </c>
+      <c r="F22" s="32">
+        <v>0</v>
+      </c>
+      <c r="G22" s="32">
+        <v>0</v>
+      </c>
+      <c r="H22" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8">
+      <c r="C23" s="34"/>
+      <c r="D23" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E23" s="32">
+        <v>0</v>
+      </c>
+      <c r="F23" s="32">
+        <v>1</v>
+      </c>
+      <c r="G23" s="32">
+        <v>0</v>
+      </c>
+      <c r="H23" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8">
+      <c r="C24" s="34"/>
+      <c r="D24" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="32">
+        <v>0</v>
+      </c>
+      <c r="F24" s="32">
+        <v>0</v>
+      </c>
+      <c r="G24" s="32">
+        <v>2</v>
+      </c>
+      <c r="H24" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8">
+      <c r="C25" s="38"/>
+      <c r="D25" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E25" s="32">
+        <v>0</v>
+      </c>
+      <c r="F25" s="32">
+        <v>0</v>
+      </c>
+      <c r="G25" s="32">
+        <v>0</v>
+      </c>
+      <c r="H25" s="32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8">
+      <c r="A27" s="18">
+        <v>3</v>
+      </c>
+      <c r="B27" t="s">
+        <v>47</v>
+      </c>
+      <c r="C27" s="27"/>
+      <c r="D27" s="28"/>
+      <c r="E27" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F27" s="29"/>
+      <c r="G27" s="29"/>
+      <c r="H27" s="30"/>
+    </row>
+    <row r="28" spans="1:8">
+      <c r="C28" s="31"/>
+      <c r="D28" s="32"/>
+      <c r="E28" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="F28" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G28" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="H28" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8">
+      <c r="C29" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D29" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="32">
+        <v>1</v>
+      </c>
+      <c r="F29" s="32">
+        <v>0</v>
+      </c>
+      <c r="G29" s="32">
+        <v>0</v>
+      </c>
+      <c r="H29" s="32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8">
+      <c r="C30" s="34"/>
+      <c r="D30" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E30" s="32">
+        <v>0</v>
+      </c>
+      <c r="F30" s="32">
+        <v>1</v>
+      </c>
+      <c r="G30" s="32">
+        <v>0</v>
+      </c>
+      <c r="H30" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8">
+      <c r="C31" s="34"/>
+      <c r="D31" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E31" s="32">
+        <v>0</v>
+      </c>
+      <c r="F31" s="32">
+        <v>0</v>
+      </c>
+      <c r="G31" s="32">
+        <v>2</v>
+      </c>
+      <c r="H31" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8">
+      <c r="C32" s="38"/>
+      <c r="D32" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E32" s="32">
+        <v>0</v>
+      </c>
+      <c r="F32" s="32">
+        <v>0</v>
+      </c>
+      <c r="G32" s="32">
+        <v>0</v>
+      </c>
+      <c r="H32" s="32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8">
+      <c r="A34" s="18">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>50</v>
+      </c>
+      <c r="C34" s="27"/>
+      <c r="D34" s="28"/>
+      <c r="E34" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F34" s="29"/>
+      <c r="G34" s="29"/>
+      <c r="H34" s="30"/>
+    </row>
+    <row r="35" spans="1:8">
+      <c r="C35" s="31"/>
+      <c r="D35" s="32"/>
+      <c r="E35" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="F35" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="H35" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8">
+      <c r="C36" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D36" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="32">
+        <v>1</v>
+      </c>
+      <c r="F36" s="32">
+        <v>0</v>
+      </c>
+      <c r="G36" s="32">
+        <v>0</v>
+      </c>
+      <c r="H36" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8">
+      <c r="C37" s="34"/>
+      <c r="D37" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="32">
+        <v>0</v>
+      </c>
+      <c r="F37" s="32">
+        <v>2</v>
+      </c>
+      <c r="G37" s="32">
+        <v>0</v>
+      </c>
+      <c r="H37" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8">
+      <c r="C38" s="34"/>
+      <c r="D38" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E38" s="32">
+        <v>0</v>
+      </c>
+      <c r="F38" s="32">
+        <v>0</v>
+      </c>
+      <c r="G38" s="32">
+        <v>1</v>
+      </c>
+      <c r="H38" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8">
+      <c r="C39" s="38"/>
+      <c r="D39" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E39" s="32">
+        <v>0</v>
+      </c>
+      <c r="F39" s="32">
+        <v>0</v>
+      </c>
+      <c r="G39" s="32">
+        <v>0</v>
+      </c>
+      <c r="H39" s="32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8">
+      <c r="A41" s="18">
+        <v>5</v>
+      </c>
+      <c r="B41" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="C41" s="27"/>
+      <c r="D41" s="28"/>
+      <c r="E41" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F41" s="29"/>
+      <c r="G41" s="29"/>
+      <c r="H41" s="30"/>
+    </row>
+    <row r="42" spans="1:8">
+      <c r="C42" s="31"/>
+      <c r="D42" s="32"/>
+      <c r="E42" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="F42" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="H42" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8">
+      <c r="C43" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D43" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E43" s="32">
+        <v>1</v>
+      </c>
+      <c r="F43" s="32">
+        <v>0</v>
+      </c>
+      <c r="G43" s="32">
+        <v>0</v>
+      </c>
+      <c r="H43" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8">
+      <c r="C44" s="34"/>
+      <c r="D44" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E44" s="32">
+        <v>0</v>
+      </c>
+      <c r="F44" s="32">
+        <v>2</v>
+      </c>
+      <c r="G44" s="32">
+        <v>0</v>
+      </c>
+      <c r="H44" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8">
+      <c r="C45" s="34"/>
+      <c r="D45" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E45" s="32">
+        <v>0</v>
+      </c>
+      <c r="F45" s="32">
+        <v>0</v>
+      </c>
+      <c r="G45" s="32">
+        <v>2</v>
+      </c>
+      <c r="H45" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8">
+      <c r="C46" s="38"/>
+      <c r="D46" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E46" s="32">
+        <v>0</v>
+      </c>
+      <c r="F46" s="32">
+        <v>0</v>
+      </c>
+      <c r="G46" s="32">
+        <v>0</v>
+      </c>
+      <c r="H46" s="32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8">
+      <c r="A48" s="18">
+        <v>6</v>
+      </c>
+      <c r="B48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C48" s="27"/>
+      <c r="D48" s="28"/>
+      <c r="E48" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F48" s="29"/>
+      <c r="G48" s="29"/>
+      <c r="H48" s="30"/>
+    </row>
+    <row r="49" spans="1:8">
+      <c r="C49" s="31"/>
+      <c r="D49" s="32"/>
+      <c r="E49" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="F49" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G49" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="H49" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8">
+      <c r="C50" s="34" t="s">
+        <v>25</v>
+      </c>
+      <c r="D50" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E50" s="32">
+        <v>1</v>
+      </c>
+      <c r="F50" s="32">
+        <v>0</v>
+      </c>
+      <c r="G50" s="32">
+        <v>0</v>
+      </c>
+      <c r="H50" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:8">
+      <c r="C51" s="34"/>
+      <c r="D51" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E51" s="32">
+        <v>0</v>
+      </c>
+      <c r="F51" s="32">
+        <v>2</v>
+      </c>
+      <c r="G51" s="32">
+        <v>0</v>
+      </c>
+      <c r="H51" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:8">
+      <c r="C52" s="34"/>
+      <c r="D52" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E52" s="32">
+        <v>0</v>
+      </c>
+      <c r="F52" s="32">
+        <v>0</v>
+      </c>
+      <c r="G52" s="32">
+        <v>1</v>
+      </c>
+      <c r="H52" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:8">
+      <c r="C53" s="38"/>
+      <c r="D53" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E53" s="32">
+        <v>0</v>
+      </c>
+      <c r="F53" s="32">
+        <v>0</v>
+      </c>
+      <c r="G53" s="32">
+        <v>0</v>
+      </c>
+      <c r="H53" s="32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="55" spans="1:8">
+      <c r="A55" s="18">
+        <v>6</v>
+      </c>
+      <c r="B55" t="s">
+        <v>51</v>
+      </c>
+      <c r="C55" s="27"/>
+      <c r="D55" s="28"/>
+      <c r="E55" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="F55" s="29"/>
+      <c r="G55" s="29"/>
+      <c r="H55" s="30"/>
+    </row>
+    <row r="56" spans="1:8">
+      <c r="C56" s="31"/>
+      <c r="D56" s="32"/>
+      <c r="E56" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="F56" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G56" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="H56" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="57" spans="1:8">
+      <c r="C57" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D57" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E57" s="32">
+        <v>3</v>
+      </c>
+      <c r="F57" s="32">
+        <v>0</v>
+      </c>
+      <c r="G57" s="32">
+        <v>0</v>
+      </c>
+      <c r="H57" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:8">
+      <c r="C58" s="35"/>
+      <c r="D58" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E58" s="32">
+        <v>0</v>
+      </c>
+      <c r="F58" s="32">
+        <v>1</v>
+      </c>
+      <c r="G58" s="32">
+        <v>0</v>
+      </c>
+      <c r="H58" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:8">
+      <c r="C59" s="35"/>
+      <c r="D59" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E59" s="32">
+        <v>0</v>
+      </c>
+      <c r="F59" s="32">
+        <v>0</v>
+      </c>
+      <c r="G59" s="32">
+        <v>1</v>
+      </c>
+      <c r="H59" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:8">
+      <c r="C60" s="36"/>
+      <c r="D60" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E60" s="32">
+        <v>0</v>
+      </c>
+      <c r="F60" s="32">
+        <v>0</v>
+      </c>
+      <c r="G60" s="32">
+        <v>0</v>
+      </c>
+      <c r="H60" s="32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="62" spans="1:8">
+      <c r="A62" s="18">
+        <v>7</v>
+      </c>
+      <c r="B62" t="s">
+        <v>52</v>
+      </c>
+      <c r="C62" s="27"/>
+      <c r="D62" s="28"/>
+      <c r="E62" s="29" t="s">
+        <v>24</v>
+      </c>
+      <c r="F62" s="29"/>
+      <c r="G62" s="29"/>
+      <c r="H62" s="30"/>
+    </row>
+    <row r="63" spans="1:8">
+      <c r="C63" s="31"/>
+      <c r="D63" s="32"/>
+      <c r="E63" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="F63" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G63" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="H63" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="64" spans="1:8">
+      <c r="C64" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D64" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E64" s="32">
+        <v>2</v>
+      </c>
+      <c r="F64" s="32">
+        <v>0</v>
+      </c>
+      <c r="G64" s="32">
+        <v>0</v>
+      </c>
+      <c r="H64" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:8">
+      <c r="C65" s="35"/>
+      <c r="D65" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E65" s="32">
+        <v>0</v>
+      </c>
+      <c r="F65" s="32">
+        <v>0</v>
+      </c>
+      <c r="G65" s="32">
+        <v>0</v>
+      </c>
+      <c r="H65" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:8">
+      <c r="C66" s="35"/>
+      <c r="D66" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E66" s="32">
+        <v>0</v>
+      </c>
+      <c r="F66" s="32">
+        <v>0</v>
+      </c>
+      <c r="G66" s="32">
+        <v>2</v>
+      </c>
+      <c r="H66" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:8">
+      <c r="C67" s="36"/>
+      <c r="D67" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E67" s="32">
+        <v>0</v>
+      </c>
+      <c r="F67" s="32">
+        <v>0</v>
+      </c>
+      <c r="G67" s="32">
+        <v>0</v>
+      </c>
+      <c r="H67" s="32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="69" spans="1:8">
+      <c r="A69" s="18">
+        <v>8</v>
+      </c>
+      <c r="B69" t="s">
+        <v>53</v>
+      </c>
+      <c r="C69" s="27"/>
+      <c r="D69" s="28"/>
+      <c r="E69" s="29" t="s">
+        <v>62</v>
+      </c>
+      <c r="F69" s="29"/>
+      <c r="G69" s="29"/>
+      <c r="H69" s="30"/>
+    </row>
+    <row r="70" spans="1:8">
+      <c r="C70" s="31"/>
+      <c r="D70" s="32"/>
+      <c r="E70" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="F70" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="G70" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="H70" s="33" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="71" spans="1:8">
+      <c r="C71" s="35" t="s">
+        <v>25</v>
+      </c>
+      <c r="D71" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="E71" s="32">
+        <v>1</v>
+      </c>
+      <c r="F71" s="32">
+        <v>0</v>
+      </c>
+      <c r="G71" s="32">
+        <v>0</v>
+      </c>
+      <c r="H71" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:8">
+      <c r="C72" s="35"/>
+      <c r="D72" s="33" t="s">
+        <v>4</v>
+      </c>
+      <c r="E72" s="32">
+        <v>0</v>
+      </c>
+      <c r="F72" s="32">
+        <v>2</v>
+      </c>
+      <c r="G72" s="32">
+        <v>0</v>
+      </c>
+      <c r="H72" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:8">
+      <c r="C73" s="35"/>
+      <c r="D73" s="33" t="s">
+        <v>18</v>
+      </c>
+      <c r="E73" s="32">
+        <v>0</v>
+      </c>
+      <c r="F73" s="32">
+        <v>0</v>
+      </c>
+      <c r="G73" s="32">
+        <v>1</v>
+      </c>
+      <c r="H73" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:8">
+      <c r="C74" s="36"/>
+      <c r="D74" s="33" t="s">
+        <v>22</v>
+      </c>
+      <c r="E74" s="32">
+        <v>0</v>
+      </c>
+      <c r="F74" s="32">
+        <v>0</v>
+      </c>
+      <c r="G74" s="32">
+        <v>0</v>
+      </c>
+      <c r="H74" s="32">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2">
+      <c r="B116" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2">
+      <c r="B117" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="118" spans="2:2">
+      <c r="B118" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="119" spans="2:2">
+      <c r="B119" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2">
+      <c r="B120" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2">
+      <c r="B121" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2">
+      <c r="B122" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2">
+      <c r="B123" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2">
+      <c r="B124" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2">
+      <c r="B125" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2">
+      <c r="B126" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2">
+      <c r="B127" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2">
+      <c r="B128" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2">
+      <c r="B129" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2">
+      <c r="B130" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2">
+      <c r="B131" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2">
+      <c r="B132" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2">
+      <c r="B133" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2">
+      <c r="B134" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2">
+      <c r="B135" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2">
+      <c r="B136" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2">
+      <c r="B137" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2">
+      <c r="B138" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2">
+      <c r="B139" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2">
+      <c r="B140" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2">
+      <c r="B141" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2">
+      <c r="B142" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C71:C74"/>
+    <mergeCell ref="C57:C60"/>
+    <mergeCell ref="C64:C67"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:8">
+      <c r="B1" s="10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
+      <c r="H1" s="26"/>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="B2" s="10"/>
+      <c r="C2" s="21"/>
+      <c r="D2" s="19"/>
+      <c r="E2" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H2" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="B3" s="10"/>
+      <c r="C3" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="19"/>
+      <c r="F3" s="19"/>
+      <c r="G3" s="19"/>
+      <c r="H3" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="B4" s="10"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E4" s="19"/>
+      <c r="F4" s="19">
+        <v>2</v>
+      </c>
+      <c r="G4" s="19"/>
+      <c r="H4" s="19"/>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="B5" s="10"/>
+      <c r="C5" s="22"/>
+      <c r="D5" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="19">
+        <v>1</v>
+      </c>
+      <c r="F5" s="19"/>
+      <c r="G5" s="19">
+        <v>1</v>
+      </c>
+      <c r="H5" s="19"/>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="B6" s="10"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="19"/>
+      <c r="H6" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="B7" s="10"/>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="B8" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="19"/>
+      <c r="D8" s="24"/>
+      <c r="E8" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F8" s="25"/>
+      <c r="G8" s="25"/>
+      <c r="H8" s="26"/>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="B9" s="10"/>
+      <c r="C9" s="21"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H9" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="B10" s="10"/>
+      <c r="C10" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D10" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E10" s="19"/>
+      <c r="F10" s="19"/>
+      <c r="G10" s="19"/>
+      <c r="H10" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8">
+      <c r="B11" s="10"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E11" s="19"/>
+      <c r="F11" s="19">
+        <v>2</v>
+      </c>
+      <c r="G11" s="19"/>
+      <c r="H11" s="19"/>
+    </row>
+    <row r="12" spans="1:8">
+      <c r="B12" s="10"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="19">
+        <v>1</v>
+      </c>
+      <c r="F12" s="19"/>
+      <c r="G12" s="19">
+        <v>1</v>
+      </c>
+      <c r="H12" s="19"/>
+    </row>
+    <row r="13" spans="1:8">
+      <c r="B13" s="10"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13" s="19"/>
+      <c r="F13" s="19"/>
+      <c r="G13" s="19"/>
+      <c r="H13" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8">
+      <c r="B14" s="10"/>
+    </row>
+    <row r="15" spans="1:8">
+      <c r="A15" s="18"/>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="19"/>
+      <c r="D15" s="24"/>
+      <c r="E15" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F15" s="25"/>
+      <c r="G15" s="25"/>
+      <c r="H15" s="26"/>
+    </row>
+    <row r="16" spans="1:8">
+      <c r="A16" s="18"/>
+      <c r="C16" s="21"/>
+      <c r="D16" s="19"/>
+      <c r="E16" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="F16" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="H16" s="20" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8">
+      <c r="A17" s="18"/>
+      <c r="C17" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>0</v>
+      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" s="19"/>
+      <c r="G17" s="19"/>
+      <c r="H17" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8">
+      <c r="A18" s="18"/>
+      <c r="C18" s="22"/>
+      <c r="D18" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="E18" s="19"/>
+      <c r="F18" s="19">
+        <v>2</v>
+      </c>
+      <c r="G18" s="19"/>
+      <c r="H18" s="19"/>
+    </row>
+    <row r="19" spans="1:8">
+      <c r="A19" s="18"/>
+      <c r="C19" s="22"/>
+      <c r="D19" s="20" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="19">
+        <v>1</v>
+      </c>
+      <c r="F19" s="19"/>
+      <c r="G19" s="19">
+        <v>1</v>
+      </c>
+      <c r="H19" s="19"/>
+    </row>
+    <row r="20" spans="1:8">
+      <c r="A20" s="18"/>
+      <c r="C20" s="23"/>
+      <c r="D20" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="E20" s="19"/>
+      <c r="F20" s="19"/>
+      <c r="G20" s="19"/>
+      <c r="H20" s="19">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="C3:C6"/>
+    <mergeCell ref="C10:C13"/>
+    <mergeCell ref="C17:C20"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>